<commit_message>
more factoring and geom_label
</commit_message>
<xml_diff>
--- a/dataexample.xlsx
+++ b/dataexample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19200" windowHeight="10860"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="13680" windowHeight="7440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,39 +32,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t>Flexible pricing</t>
-  </si>
-  <si>
-    <t>Mobile money</t>
-  </si>
-  <si>
-    <t>PAYG</t>
-  </si>
-  <si>
-    <t>Payment system</t>
-  </si>
-  <si>
-    <t>Financial literacy</t>
-  </si>
-  <si>
-    <t>Cost of alternatives</t>
-  </si>
-  <si>
-    <t>Tax</t>
-  </si>
-  <si>
-    <t>Loan</t>
-  </si>
-  <si>
-    <t>Banking infrastructure</t>
-  </si>
-  <si>
-    <t>Financing option</t>
-  </si>
-  <si>
-    <t>Cost to user</t>
-  </si>
-  <si>
     <t>barrier_strong</t>
   </si>
   <si>
@@ -81,6 +48,39 @@
   </si>
   <si>
     <t>driver_strong</t>
+  </si>
+  <si>
+    <t>Ropes</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Tough</t>
+  </si>
+  <si>
+    <t>Shot</t>
+  </si>
+  <si>
+    <t>Fiddle</t>
+  </si>
+  <si>
+    <t>Lickety</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Silver</t>
+  </si>
+  <si>
+    <t>Surgery</t>
+  </si>
+  <si>
+    <t>Drawing</t>
+  </si>
+  <si>
+    <t>Jumping</t>
+  </si>
+  <si>
+    <t>Sock In It</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,27 +502,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -562,7 +562,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>-2</v>
@@ -622,7 +622,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>-2</v>
@@ -642,7 +642,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>-2</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>-2</v>
@@ -682,7 +682,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>-8</v>
@@ -702,7 +702,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>-7</v>
@@ -722,7 +722,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>-21</v>

</xml_diff>